<commit_message>
new coding and guideline
</commit_message>
<xml_diff>
--- a/1.1.NC_Korea.xlsx
+++ b/1.1.NC_Korea.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://o365inha-my.sharepoint.com/personal/jshin90_office_inha_ac_kr/Documents/바탕 화면/ESG_Logistics/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="34" documentId="11_078139DD43787A0F62355476585DCE3A875EC78C" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8760EA9E-64F3-4EE5-88B0-83793105EB9C}"/>
+  <xr:revisionPtr revIDLastSave="38" documentId="11_078139DD43787A0F62355476585DCE3A875EC78C" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6E32AB07-C443-47B6-BC48-61B328A62401}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="8910" yWindow="-16200" windowWidth="19200" windowHeight="11175" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet3" sheetId="3" r:id="rId1"/>
@@ -28776,7 +28776,7 @@
   <dimension ref="A1:B455"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
@@ -36113,8 +36113,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:E2304"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="A1:E1"/>
+    <sheetView tabSelected="1" topLeftCell="A1071" workbookViewId="0">
+      <selection activeCell="A102" sqref="A102:A2211"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
@@ -37179,7 +37179,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A63" t="s">
         <v>181</v>
       </c>
@@ -37400,7 +37400,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="76" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A76" t="s">
         <v>215</v>
       </c>
@@ -37672,7 +37672,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="92" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A92" t="s">
         <v>255</v>
       </c>
@@ -37706,7 +37706,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="94" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A94" t="s">
         <v>259</v>
       </c>
@@ -37757,7 +37757,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="97" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A97" t="s">
         <v>267</v>
       </c>
@@ -37842,21 +37842,21 @@
         <v>66</v>
       </c>
     </row>
-    <row r="102" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A102" t="s">
-        <v>279</v>
+        <v>381</v>
       </c>
       <c r="B102" t="s">
-        <v>280</v>
+        <v>382</v>
       </c>
       <c r="C102" t="s">
         <v>281</v>
       </c>
       <c r="D102">
-        <v>101</v>
+        <v>142</v>
       </c>
       <c r="E102" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
     </row>
     <row r="103" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
@@ -38029,21 +38029,21 @@
         <v>7</v>
       </c>
     </row>
-    <row r="113" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
+    <row r="113" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A113" t="s">
-        <v>311</v>
+        <v>398</v>
       </c>
       <c r="B113" t="s">
-        <v>312</v>
+        <v>399</v>
       </c>
       <c r="C113" t="s">
         <v>281</v>
       </c>
       <c r="D113">
-        <v>112</v>
+        <v>149</v>
       </c>
       <c r="E113" t="s">
-        <v>40</v>
+        <v>14</v>
       </c>
     </row>
     <row r="114" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
@@ -38063,140 +38063,140 @@
         <v>7</v>
       </c>
     </row>
-    <row r="115" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
+    <row r="115" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A115" t="s">
-        <v>315</v>
+        <v>508</v>
       </c>
       <c r="B115" t="s">
-        <v>316</v>
+        <v>509</v>
       </c>
       <c r="C115" t="s">
         <v>281</v>
       </c>
       <c r="D115">
-        <v>114</v>
+        <v>193</v>
       </c>
       <c r="E115" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="116" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A116" t="s">
-        <v>317</v>
+        <v>771</v>
       </c>
       <c r="B116" t="s">
-        <v>318</v>
+        <v>772</v>
       </c>
       <c r="C116" t="s">
         <v>281</v>
       </c>
       <c r="D116">
-        <v>115</v>
+        <v>291</v>
       </c>
       <c r="E116" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="117" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A117" t="s">
-        <v>319</v>
+        <v>809</v>
       </c>
       <c r="B117" t="s">
-        <v>320</v>
+        <v>810</v>
       </c>
       <c r="C117" t="s">
         <v>281</v>
       </c>
       <c r="D117">
-        <v>116</v>
+        <v>306</v>
       </c>
       <c r="E117" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="118" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A118" t="s">
-        <v>321</v>
+        <v>4137</v>
       </c>
       <c r="B118" t="s">
-        <v>322</v>
+        <v>4138</v>
       </c>
       <c r="C118" t="s">
         <v>281</v>
       </c>
       <c r="D118">
-        <v>117</v>
+        <v>1823</v>
       </c>
       <c r="E118" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="119" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A119" t="s">
-        <v>323</v>
+        <v>761</v>
       </c>
       <c r="B119" t="s">
-        <v>324</v>
+        <v>762</v>
       </c>
       <c r="C119" t="s">
         <v>281</v>
       </c>
       <c r="D119">
-        <v>118</v>
+        <v>287</v>
       </c>
       <c r="E119" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="120" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
+        <v>763</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A120" t="s">
-        <v>325</v>
+        <v>797</v>
       </c>
       <c r="B120" t="s">
-        <v>326</v>
+        <v>798</v>
       </c>
       <c r="C120" t="s">
         <v>281</v>
       </c>
       <c r="D120">
-        <v>119</v>
+        <v>301</v>
       </c>
       <c r="E120" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="121" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
+        <v>711</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A121" t="s">
-        <v>327</v>
+        <v>1338</v>
       </c>
       <c r="B121" t="s">
-        <v>328</v>
+        <v>1339</v>
       </c>
       <c r="C121" t="s">
         <v>281</v>
       </c>
       <c r="D121">
-        <v>120</v>
+        <v>520</v>
       </c>
       <c r="E121" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="122" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
+        <v>711</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A122" t="s">
-        <v>329</v>
+        <v>1859</v>
       </c>
       <c r="B122" t="s">
-        <v>330</v>
+        <v>1860</v>
       </c>
       <c r="C122" t="s">
         <v>281</v>
       </c>
       <c r="D122">
-        <v>121</v>
+        <v>754</v>
       </c>
       <c r="E122" t="s">
-        <v>40</v>
+        <v>711</v>
       </c>
     </row>
     <row r="123" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
@@ -38250,35 +38250,35 @@
         <v>7</v>
       </c>
     </row>
-    <row r="126" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
+    <row r="126" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A126" t="s">
-        <v>340</v>
+        <v>813</v>
       </c>
       <c r="B126" t="s">
-        <v>341</v>
+        <v>814</v>
       </c>
       <c r="C126" t="s">
         <v>281</v>
       </c>
       <c r="D126">
-        <v>125</v>
+        <v>308</v>
       </c>
       <c r="E126" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="127" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
+        <v>815</v>
+      </c>
+    </row>
+    <row r="127" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A127" t="s">
-        <v>342</v>
+        <v>279</v>
       </c>
       <c r="B127" t="s">
-        <v>343</v>
+        <v>280</v>
       </c>
       <c r="C127" t="s">
         <v>281</v>
       </c>
       <c r="D127">
-        <v>126</v>
+        <v>101</v>
       </c>
       <c r="E127" t="s">
         <v>27</v>
@@ -38335,21 +38335,21 @@
         <v>89</v>
       </c>
     </row>
-    <row r="131" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
+    <row r="131" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A131" t="s">
-        <v>352</v>
+        <v>317</v>
       </c>
       <c r="B131" t="s">
-        <v>353</v>
+        <v>318</v>
       </c>
       <c r="C131" t="s">
         <v>281</v>
       </c>
       <c r="D131">
-        <v>130</v>
+        <v>115</v>
       </c>
       <c r="E131" t="s">
-        <v>47</v>
+        <v>27</v>
       </c>
     </row>
     <row r="132" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
@@ -38403,21 +38403,21 @@
         <v>27</v>
       </c>
     </row>
-    <row r="135" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
+    <row r="135" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A135" t="s">
-        <v>362</v>
+        <v>321</v>
       </c>
       <c r="B135" t="s">
-        <v>363</v>
+        <v>322</v>
       </c>
       <c r="C135" t="s">
         <v>281</v>
       </c>
       <c r="D135">
-        <v>134</v>
+        <v>117</v>
       </c>
       <c r="E135" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
     </row>
     <row r="136" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
@@ -38437,21 +38437,21 @@
         <v>122</v>
       </c>
     </row>
-    <row r="137" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
+    <row r="137" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A137" t="s">
-        <v>366</v>
+        <v>325</v>
       </c>
       <c r="B137" t="s">
-        <v>367</v>
+        <v>326</v>
       </c>
       <c r="C137" t="s">
         <v>281</v>
       </c>
       <c r="D137">
-        <v>136</v>
+        <v>119</v>
       </c>
       <c r="E137" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
     </row>
     <row r="138" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
@@ -38488,38 +38488,38 @@
         <v>47</v>
       </c>
     </row>
-    <row r="140" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
+    <row r="140" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A140" t="s">
-        <v>374</v>
+        <v>340</v>
       </c>
       <c r="B140" t="s">
-        <v>375</v>
+        <v>341</v>
       </c>
       <c r="C140" t="s">
         <v>281</v>
       </c>
       <c r="D140">
-        <v>139</v>
+        <v>125</v>
       </c>
       <c r="E140" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="141" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="141" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A141" t="s">
-        <v>376</v>
+        <v>342</v>
       </c>
       <c r="B141" t="s">
-        <v>377</v>
+        <v>343</v>
       </c>
       <c r="C141" t="s">
         <v>281</v>
       </c>
       <c r="D141">
-        <v>140</v>
+        <v>126</v>
       </c>
       <c r="E141" t="s">
-        <v>176</v>
+        <v>27</v>
       </c>
     </row>
     <row r="142" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
@@ -38539,21 +38539,21 @@
         <v>40</v>
       </c>
     </row>
-    <row r="143" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
+    <row r="143" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A143" t="s">
-        <v>381</v>
+        <v>4806</v>
       </c>
       <c r="B143" t="s">
-        <v>382</v>
+        <v>4807</v>
       </c>
       <c r="C143" t="s">
         <v>281</v>
       </c>
       <c r="D143">
-        <v>142</v>
+        <v>2143</v>
       </c>
       <c r="E143" t="s">
-        <v>14</v>
+        <v>27</v>
       </c>
     </row>
     <row r="144" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
@@ -38573,21 +38573,21 @@
         <v>40</v>
       </c>
     </row>
-    <row r="145" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
+    <row r="145" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A145" t="s">
-        <v>386</v>
+        <v>895</v>
       </c>
       <c r="B145" t="s">
-        <v>387</v>
+        <v>896</v>
       </c>
       <c r="C145" t="s">
         <v>281</v>
       </c>
       <c r="D145">
-        <v>144</v>
+        <v>340</v>
       </c>
       <c r="E145" t="s">
-        <v>176</v>
+        <v>791</v>
       </c>
     </row>
     <row r="146" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
@@ -38658,21 +38658,21 @@
         <v>47</v>
       </c>
     </row>
-    <row r="150" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
+    <row r="150" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A150" t="s">
-        <v>398</v>
+        <v>1041</v>
       </c>
       <c r="B150" t="s">
-        <v>399</v>
+        <v>1042</v>
       </c>
       <c r="C150" t="s">
         <v>281</v>
       </c>
       <c r="D150">
-        <v>149</v>
+        <v>398</v>
       </c>
       <c r="E150" t="s">
-        <v>14</v>
+        <v>791</v>
       </c>
     </row>
     <row r="151" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
@@ -38709,21 +38709,21 @@
         <v>40</v>
       </c>
     </row>
-    <row r="153" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
+    <row r="153" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A153" t="s">
-        <v>406</v>
+        <v>2548</v>
       </c>
       <c r="B153" t="s">
-        <v>407</v>
+        <v>2549</v>
       </c>
       <c r="C153" t="s">
         <v>281</v>
       </c>
       <c r="D153">
-        <v>152</v>
+        <v>1073</v>
       </c>
       <c r="E153" t="s">
-        <v>89</v>
+        <v>791</v>
       </c>
     </row>
     <row r="154" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
@@ -39015,21 +39015,21 @@
         <v>40</v>
       </c>
     </row>
-    <row r="171" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
+    <row r="171" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A171" t="s">
-        <v>450</v>
+        <v>638</v>
       </c>
       <c r="B171" t="s">
-        <v>451</v>
+        <v>639</v>
       </c>
       <c r="C171" t="s">
         <v>281</v>
       </c>
       <c r="D171">
-        <v>170</v>
+        <v>245</v>
       </c>
       <c r="E171" t="s">
-        <v>122</v>
+        <v>640</v>
       </c>
     </row>
     <row r="172" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
@@ -39117,7 +39117,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="177" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="177" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A177" t="s">
         <v>464</v>
       </c>
@@ -39134,7 +39134,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="178" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="178" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A178" t="s">
         <v>466</v>
       </c>
@@ -39287,21 +39287,21 @@
         <v>40</v>
       </c>
     </row>
-    <row r="187" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
+    <row r="187" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A187" t="s">
-        <v>490</v>
+        <v>4830</v>
       </c>
       <c r="B187" t="s">
-        <v>491</v>
+        <v>4831</v>
       </c>
       <c r="C187" t="s">
         <v>281</v>
       </c>
       <c r="D187">
-        <v>186</v>
+        <v>2155</v>
       </c>
       <c r="E187" t="s">
-        <v>484</v>
+        <v>640</v>
       </c>
     </row>
     <row r="188" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
@@ -39406,21 +39406,21 @@
         <v>66</v>
       </c>
     </row>
-    <row r="194" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
+    <row r="194" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A194" t="s">
-        <v>508</v>
+        <v>3109</v>
       </c>
       <c r="B194" t="s">
-        <v>509</v>
+        <v>3110</v>
       </c>
       <c r="C194" t="s">
         <v>281</v>
       </c>
       <c r="D194">
-        <v>193</v>
+        <v>1337</v>
       </c>
       <c r="E194" t="s">
-        <v>14</v>
+        <v>832</v>
       </c>
     </row>
     <row r="195" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
@@ -39712,21 +39712,21 @@
         <v>89</v>
       </c>
     </row>
-    <row r="212" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
+    <row r="212" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A212" t="s">
-        <v>551</v>
+        <v>3111</v>
       </c>
       <c r="B212" t="s">
-        <v>552</v>
+        <v>3112</v>
       </c>
       <c r="C212" t="s">
         <v>281</v>
       </c>
       <c r="D212">
-        <v>211</v>
+        <v>1338</v>
       </c>
       <c r="E212" t="s">
-        <v>176</v>
+        <v>832</v>
       </c>
     </row>
     <row r="213" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
@@ -39746,21 +39746,21 @@
         <v>197</v>
       </c>
     </row>
-    <row r="214" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
+    <row r="214" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A214" t="s">
-        <v>555</v>
+        <v>4155</v>
       </c>
       <c r="B214" t="s">
-        <v>556</v>
+        <v>4156</v>
       </c>
       <c r="C214" t="s">
         <v>281</v>
       </c>
       <c r="D214">
-        <v>213</v>
+        <v>1832</v>
       </c>
       <c r="E214" t="s">
-        <v>197</v>
+        <v>832</v>
       </c>
     </row>
     <row r="215" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
@@ -39882,21 +39882,21 @@
         <v>66</v>
       </c>
     </row>
-    <row r="222" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
+    <row r="222" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A222" t="s">
-        <v>574</v>
+        <v>2093</v>
       </c>
       <c r="B222" t="s">
-        <v>575</v>
+        <v>2094</v>
       </c>
       <c r="C222" t="s">
         <v>281</v>
       </c>
       <c r="D222">
-        <v>221</v>
+        <v>860</v>
       </c>
       <c r="E222" t="s">
-        <v>576</v>
+        <v>977</v>
       </c>
     </row>
     <row r="223" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
@@ -39950,38 +39950,38 @@
         <v>584</v>
       </c>
     </row>
-    <row r="226" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
+    <row r="226" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A226" t="s">
-        <v>585</v>
+        <v>3515</v>
       </c>
       <c r="B226" t="s">
-        <v>586</v>
+        <v>3516</v>
       </c>
       <c r="C226" t="s">
         <v>281</v>
       </c>
       <c r="D226">
-        <v>225</v>
+        <v>1530</v>
       </c>
       <c r="E226" t="s">
-        <v>587</v>
-      </c>
-    </row>
-    <row r="227" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
+        <v>1003</v>
+      </c>
+    </row>
+    <row r="227" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A227" t="s">
-        <v>588</v>
+        <v>1429</v>
       </c>
       <c r="B227" t="s">
-        <v>589</v>
+        <v>1430</v>
       </c>
       <c r="C227" t="s">
         <v>281</v>
       </c>
       <c r="D227">
-        <v>226</v>
+        <v>562</v>
       </c>
       <c r="E227" t="s">
-        <v>590</v>
+        <v>1431</v>
       </c>
     </row>
     <row r="228" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
@@ -40001,21 +40001,21 @@
         <v>197</v>
       </c>
     </row>
-    <row r="229" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
+    <row r="229" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A229" t="s">
-        <v>593</v>
+        <v>311</v>
       </c>
       <c r="B229" t="s">
-        <v>594</v>
+        <v>312</v>
       </c>
       <c r="C229" t="s">
         <v>281</v>
       </c>
       <c r="D229">
-        <v>228</v>
+        <v>112</v>
       </c>
       <c r="E229" t="s">
-        <v>587</v>
+        <v>40</v>
       </c>
     </row>
     <row r="230" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
@@ -40086,38 +40086,38 @@
         <v>606</v>
       </c>
     </row>
-    <row r="234" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
+    <row r="234" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A234" t="s">
-        <v>574</v>
+        <v>329</v>
       </c>
       <c r="B234" t="s">
-        <v>607</v>
+        <v>330</v>
       </c>
       <c r="C234" t="s">
         <v>281</v>
       </c>
       <c r="D234">
-        <v>233</v>
+        <v>121</v>
       </c>
       <c r="E234" t="s">
-        <v>576</v>
-      </c>
-    </row>
-    <row r="235" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="235" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A235" t="s">
-        <v>608</v>
+        <v>362</v>
       </c>
       <c r="B235" t="s">
-        <v>609</v>
+        <v>363</v>
       </c>
       <c r="C235" t="s">
         <v>281</v>
       </c>
       <c r="D235">
-        <v>234</v>
+        <v>134</v>
       </c>
       <c r="E235" t="s">
-        <v>610</v>
+        <v>40</v>
       </c>
     </row>
     <row r="236" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
@@ -40205,21 +40205,21 @@
         <v>624</v>
       </c>
     </row>
-    <row r="241" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
+    <row r="241" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A241" t="s">
-        <v>625</v>
+        <v>366</v>
       </c>
       <c r="B241" t="s">
-        <v>626</v>
+        <v>367</v>
       </c>
       <c r="C241" t="s">
         <v>281</v>
       </c>
       <c r="D241">
-        <v>240</v>
+        <v>136</v>
       </c>
       <c r="E241" t="s">
-        <v>597</v>
+        <v>40</v>
       </c>
     </row>
     <row r="242" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
@@ -40273,38 +40273,38 @@
         <v>634</v>
       </c>
     </row>
-    <row r="245" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
+    <row r="245" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A245" t="s">
-        <v>635</v>
+        <v>374</v>
       </c>
       <c r="B245" t="s">
-        <v>636</v>
+        <v>375</v>
       </c>
       <c r="C245" t="s">
         <v>281</v>
       </c>
       <c r="D245">
-        <v>244</v>
+        <v>139</v>
       </c>
       <c r="E245" t="s">
-        <v>637</v>
-      </c>
-    </row>
-    <row r="246" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="246" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A246" t="s">
-        <v>638</v>
+        <v>1294</v>
       </c>
       <c r="B246" t="s">
-        <v>639</v>
+        <v>1295</v>
       </c>
       <c r="C246" t="s">
         <v>281</v>
       </c>
       <c r="D246">
-        <v>245</v>
+        <v>500</v>
       </c>
       <c r="E246" t="s">
-        <v>640</v>
+        <v>40</v>
       </c>
     </row>
     <row r="247" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
@@ -40341,7 +40341,7 @@
         <v>645</v>
       </c>
     </row>
-    <row r="249" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="249" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A249" t="s">
         <v>646</v>
       </c>
@@ -40358,21 +40358,21 @@
         <v>600</v>
       </c>
     </row>
-    <row r="250" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
+    <row r="250" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A250" t="s">
-        <v>648</v>
+        <v>1817</v>
       </c>
       <c r="B250" t="s">
-        <v>649</v>
+        <v>1818</v>
       </c>
       <c r="C250" t="s">
         <v>281</v>
       </c>
       <c r="D250">
-        <v>249</v>
+        <v>733</v>
       </c>
       <c r="E250" t="s">
-        <v>650</v>
+        <v>40</v>
       </c>
     </row>
     <row r="251" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
@@ -40409,38 +40409,38 @@
         <v>656</v>
       </c>
     </row>
-    <row r="253" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
+    <row r="253" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A253" t="s">
-        <v>657</v>
+        <v>1826</v>
       </c>
       <c r="B253" t="s">
-        <v>658</v>
+        <v>1827</v>
       </c>
       <c r="C253" t="s">
         <v>281</v>
       </c>
       <c r="D253">
-        <v>252</v>
+        <v>738</v>
       </c>
       <c r="E253" t="s">
-        <v>659</v>
-      </c>
-    </row>
-    <row r="254" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="254" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A254" t="s">
-        <v>660</v>
+        <v>867</v>
       </c>
       <c r="B254" t="s">
-        <v>661</v>
+        <v>868</v>
       </c>
       <c r="C254" t="s">
         <v>281</v>
       </c>
       <c r="D254">
-        <v>253</v>
+        <v>328</v>
       </c>
       <c r="E254" t="s">
-        <v>662</v>
+        <v>668</v>
       </c>
     </row>
     <row r="255" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
@@ -40460,7 +40460,7 @@
         <v>665</v>
       </c>
     </row>
-    <row r="256" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="256" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A256" t="s">
         <v>666</v>
       </c>
@@ -40987,7 +40987,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="287" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="287" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A287" t="s">
         <v>759</v>
       </c>
@@ -41004,21 +41004,21 @@
         <v>484</v>
       </c>
     </row>
-    <row r="288" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
+    <row r="288" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A288" t="s">
-        <v>761</v>
+        <v>1936</v>
       </c>
       <c r="B288" t="s">
-        <v>762</v>
+        <v>1937</v>
       </c>
       <c r="C288" t="s">
         <v>281</v>
       </c>
       <c r="D288">
-        <v>287</v>
+        <v>788</v>
       </c>
       <c r="E288" t="s">
-        <v>763</v>
+        <v>668</v>
       </c>
     </row>
     <row r="289" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
@@ -41072,21 +41072,21 @@
         <v>176</v>
       </c>
     </row>
-    <row r="292" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
+    <row r="292" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A292" t="s">
-        <v>771</v>
+        <v>1357</v>
       </c>
       <c r="B292" t="s">
-        <v>772</v>
+        <v>1358</v>
       </c>
       <c r="C292" t="s">
         <v>281</v>
       </c>
       <c r="D292">
-        <v>291</v>
+        <v>528</v>
       </c>
       <c r="E292" t="s">
-        <v>14</v>
+        <v>708</v>
       </c>
     </row>
     <row r="293" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
@@ -41208,191 +41208,191 @@
         <v>791</v>
       </c>
     </row>
-    <row r="300" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
+    <row r="300" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A300" t="s">
-        <v>792</v>
+        <v>1401</v>
       </c>
       <c r="B300" t="s">
-        <v>793</v>
+        <v>1402</v>
       </c>
       <c r="C300" t="s">
         <v>281</v>
       </c>
       <c r="D300">
-        <v>299</v>
+        <v>549</v>
       </c>
       <c r="E300" t="s">
-        <v>597</v>
-      </c>
-    </row>
-    <row r="301" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
+        <v>708</v>
+      </c>
+    </row>
+    <row r="301" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A301" t="s">
-        <v>794</v>
+        <v>2151</v>
       </c>
       <c r="B301" t="s">
-        <v>795</v>
+        <v>2152</v>
       </c>
       <c r="C301" t="s">
         <v>281</v>
       </c>
       <c r="D301">
-        <v>300</v>
+        <v>888</v>
       </c>
       <c r="E301" t="s">
-        <v>796</v>
-      </c>
-    </row>
-    <row r="302" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
+        <v>708</v>
+      </c>
+    </row>
+    <row r="302" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A302" t="s">
-        <v>797</v>
+        <v>2186</v>
       </c>
       <c r="B302" t="s">
-        <v>798</v>
+        <v>2187</v>
       </c>
       <c r="C302" t="s">
         <v>281</v>
       </c>
       <c r="D302">
-        <v>301</v>
+        <v>904</v>
       </c>
       <c r="E302" t="s">
-        <v>711</v>
-      </c>
-    </row>
-    <row r="303" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
+        <v>708</v>
+      </c>
+    </row>
+    <row r="303" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A303" t="s">
-        <v>799</v>
+        <v>4073</v>
       </c>
       <c r="B303" t="s">
-        <v>800</v>
+        <v>4074</v>
       </c>
       <c r="C303" t="s">
         <v>281</v>
       </c>
       <c r="D303">
-        <v>302</v>
+        <v>1791</v>
       </c>
       <c r="E303" t="s">
-        <v>678</v>
-      </c>
-    </row>
-    <row r="304" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
+        <v>708</v>
+      </c>
+    </row>
+    <row r="304" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A304" t="s">
-        <v>801</v>
+        <v>2529</v>
       </c>
       <c r="B304" t="s">
-        <v>802</v>
+        <v>2530</v>
       </c>
       <c r="C304" t="s">
         <v>281</v>
       </c>
       <c r="D304">
-        <v>303</v>
+        <v>1064</v>
       </c>
       <c r="E304" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="305" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
+        <v>920</v>
+      </c>
+    </row>
+    <row r="305" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A305" t="s">
-        <v>803</v>
+        <v>1316</v>
       </c>
       <c r="B305" t="s">
-        <v>804</v>
+        <v>1317</v>
       </c>
       <c r="C305" t="s">
         <v>281</v>
       </c>
       <c r="D305">
-        <v>304</v>
+        <v>510</v>
       </c>
       <c r="E305" t="s">
-        <v>805</v>
-      </c>
-    </row>
-    <row r="306" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="306" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A306" t="s">
-        <v>806</v>
+        <v>1923</v>
       </c>
       <c r="B306" t="s">
-        <v>807</v>
+        <v>1924</v>
       </c>
       <c r="C306" t="s">
         <v>281</v>
       </c>
       <c r="D306">
-        <v>305</v>
+        <v>782</v>
       </c>
       <c r="E306" t="s">
-        <v>808</v>
-      </c>
-    </row>
-    <row r="307" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="307" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A307" t="s">
-        <v>809</v>
+        <v>2082</v>
       </c>
       <c r="B307" t="s">
-        <v>810</v>
+        <v>2083</v>
       </c>
       <c r="C307" t="s">
         <v>281</v>
       </c>
       <c r="D307">
-        <v>306</v>
+        <v>854</v>
       </c>
       <c r="E307" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="308" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="308" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A308" t="s">
-        <v>811</v>
+        <v>2527</v>
       </c>
       <c r="B308" t="s">
-        <v>812</v>
+        <v>2528</v>
       </c>
       <c r="C308" t="s">
         <v>281</v>
       </c>
       <c r="D308">
-        <v>307</v>
+        <v>1063</v>
       </c>
       <c r="E308" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="309" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="309" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A309" t="s">
-        <v>813</v>
+        <v>3362</v>
       </c>
       <c r="B309" t="s">
-        <v>814</v>
+        <v>3363</v>
       </c>
       <c r="C309" t="s">
         <v>281</v>
       </c>
       <c r="D309">
-        <v>308</v>
+        <v>1455</v>
       </c>
       <c r="E309" t="s">
-        <v>815</v>
-      </c>
-    </row>
-    <row r="310" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="310" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A310" t="s">
-        <v>816</v>
+        <v>4048</v>
       </c>
       <c r="B310" t="s">
-        <v>817</v>
+        <v>4049</v>
       </c>
       <c r="C310" t="s">
         <v>281</v>
       </c>
       <c r="D310">
-        <v>309</v>
+        <v>1779</v>
       </c>
       <c r="E310" t="s">
-        <v>818</v>
+        <v>66</v>
       </c>
     </row>
     <row r="311" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
@@ -41429,38 +41429,38 @@
         <v>650</v>
       </c>
     </row>
-    <row r="313" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
+    <row r="313" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A313" t="s">
-        <v>825</v>
+        <v>4139</v>
       </c>
       <c r="B313" t="s">
-        <v>826</v>
+        <v>4140</v>
       </c>
       <c r="C313" t="s">
         <v>281</v>
       </c>
       <c r="D313">
-        <v>312</v>
+        <v>1824</v>
       </c>
       <c r="E313" t="s">
-        <v>808</v>
-      </c>
-    </row>
-    <row r="314" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="314" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A314" t="s">
-        <v>827</v>
+        <v>1965</v>
       </c>
       <c r="B314" t="s">
-        <v>828</v>
+        <v>1966</v>
       </c>
       <c r="C314" t="s">
         <v>281</v>
       </c>
       <c r="D314">
-        <v>313</v>
+        <v>802</v>
       </c>
       <c r="E314" t="s">
-        <v>829</v>
+        <v>1967</v>
       </c>
     </row>
     <row r="315" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
@@ -41667,7 +41667,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="327" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="327" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A327" t="s">
         <v>861</v>
       </c>
@@ -41701,21 +41701,21 @@
         <v>866</v>
       </c>
     </row>
-    <row r="329" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
+    <row r="329" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A329" t="s">
-        <v>867</v>
+        <v>3068</v>
       </c>
       <c r="B329" t="s">
-        <v>868</v>
+        <v>3069</v>
       </c>
       <c r="C329" t="s">
         <v>281</v>
       </c>
       <c r="D329">
-        <v>328</v>
+        <v>1318</v>
       </c>
       <c r="E329" t="s">
-        <v>668</v>
+        <v>1078</v>
       </c>
     </row>
     <row r="330" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
@@ -41803,21 +41803,21 @@
         <v>701</v>
       </c>
     </row>
-    <row r="335" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
+    <row r="335" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A335" t="s">
-        <v>881</v>
+        <v>3536</v>
       </c>
       <c r="B335" t="s">
-        <v>882</v>
+        <v>3537</v>
       </c>
       <c r="C335" t="s">
         <v>281</v>
       </c>
       <c r="D335">
-        <v>334</v>
+        <v>1540</v>
       </c>
       <c r="E335" t="s">
-        <v>247</v>
+        <v>618</v>
       </c>
     </row>
     <row r="336" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
@@ -41837,21 +41837,21 @@
         <v>176</v>
       </c>
     </row>
-    <row r="337" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
+    <row r="337" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A337" t="s">
-        <v>885</v>
+        <v>4069</v>
       </c>
       <c r="B337" t="s">
-        <v>886</v>
+        <v>4070</v>
       </c>
       <c r="C337" t="s">
         <v>281</v>
       </c>
       <c r="D337">
-        <v>336</v>
+        <v>1789</v>
       </c>
       <c r="E337" t="s">
-        <v>701</v>
+        <v>618</v>
       </c>
     </row>
     <row r="338" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
@@ -41888,38 +41888,38 @@
         <v>89</v>
       </c>
     </row>
-    <row r="340" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
+    <row r="340" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A340" t="s">
-        <v>893</v>
+        <v>965</v>
       </c>
       <c r="B340" t="s">
-        <v>894</v>
+        <v>966</v>
       </c>
       <c r="C340" t="s">
         <v>281</v>
       </c>
       <c r="D340">
-        <v>339</v>
+        <v>368</v>
       </c>
       <c r="E340" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="341" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
+        <v>967</v>
+      </c>
+    </row>
+    <row r="341" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A341" t="s">
-        <v>895</v>
+        <v>2087</v>
       </c>
       <c r="B341" t="s">
-        <v>896</v>
+        <v>2088</v>
       </c>
       <c r="C341" t="s">
         <v>281</v>
       </c>
       <c r="D341">
-        <v>340</v>
+        <v>857</v>
       </c>
       <c r="E341" t="s">
-        <v>791</v>
+        <v>967</v>
       </c>
     </row>
     <row r="342" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
@@ -42024,21 +42024,21 @@
         <v>678</v>
       </c>
     </row>
-    <row r="348" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
+    <row r="348" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A348" t="s">
-        <v>913</v>
+        <v>574</v>
       </c>
       <c r="B348" t="s">
-        <v>914</v>
+        <v>575</v>
       </c>
       <c r="C348" t="s">
         <v>281</v>
       </c>
       <c r="D348">
-        <v>347</v>
+        <v>221</v>
       </c>
       <c r="E348" t="s">
-        <v>659</v>
+        <v>576</v>
       </c>
     </row>
     <row r="349" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
@@ -42177,21 +42177,21 @@
         <v>866</v>
       </c>
     </row>
-    <row r="357" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
+    <row r="357" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A357" t="s">
-        <v>935</v>
+        <v>574</v>
       </c>
       <c r="B357" t="s">
-        <v>936</v>
+        <v>607</v>
       </c>
       <c r="C357" t="s">
         <v>281</v>
       </c>
       <c r="D357">
-        <v>356</v>
+        <v>233</v>
       </c>
       <c r="E357" t="s">
-        <v>197</v>
+        <v>576</v>
       </c>
     </row>
     <row r="358" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
@@ -42296,21 +42296,21 @@
         <v>600</v>
       </c>
     </row>
-    <row r="364" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
+    <row r="364" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A364" t="s">
-        <v>952</v>
+        <v>3950</v>
       </c>
       <c r="B364" t="s">
-        <v>953</v>
+        <v>3951</v>
       </c>
       <c r="C364" t="s">
         <v>281</v>
       </c>
       <c r="D364">
-        <v>363</v>
+        <v>1733</v>
       </c>
       <c r="E364" t="s">
-        <v>717</v>
+        <v>576</v>
       </c>
     </row>
     <row r="365" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
@@ -42347,21 +42347,21 @@
         <v>618</v>
       </c>
     </row>
-    <row r="367" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
+    <row r="367" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A367" t="s">
-        <v>959</v>
+        <v>816</v>
       </c>
       <c r="B367" t="s">
-        <v>960</v>
+        <v>817</v>
       </c>
       <c r="C367" t="s">
         <v>281</v>
       </c>
       <c r="D367">
-        <v>366</v>
+        <v>309</v>
       </c>
       <c r="E367" t="s">
-        <v>961</v>
+        <v>818</v>
       </c>
     </row>
     <row r="368" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
@@ -42381,21 +42381,21 @@
         <v>197</v>
       </c>
     </row>
-    <row r="369" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
+    <row r="369" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A369" t="s">
-        <v>965</v>
+        <v>555</v>
       </c>
       <c r="B369" t="s">
-        <v>966</v>
+        <v>556</v>
       </c>
       <c r="C369" t="s">
         <v>281</v>
       </c>
       <c r="D369">
-        <v>368</v>
+        <v>213</v>
       </c>
       <c r="E369" t="s">
-        <v>967</v>
+        <v>197</v>
       </c>
     </row>
     <row r="370" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
@@ -42738,7 +42738,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="390" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="390" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A390" t="s">
         <v>1020</v>
       </c>
@@ -42891,21 +42891,21 @@
         <v>1009</v>
       </c>
     </row>
-    <row r="399" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
+    <row r="399" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A399" t="s">
-        <v>1041</v>
+        <v>811</v>
       </c>
       <c r="B399" t="s">
-        <v>1042</v>
+        <v>812</v>
       </c>
       <c r="C399" t="s">
         <v>281</v>
       </c>
       <c r="D399">
-        <v>398</v>
+        <v>307</v>
       </c>
       <c r="E399" t="s">
-        <v>791</v>
+        <v>197</v>
       </c>
     </row>
     <row r="400" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
@@ -43673,21 +43673,21 @@
         <v>905</v>
       </c>
     </row>
-    <row r="445" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
+    <row r="445" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A445" t="s">
-        <v>1156</v>
+        <v>935</v>
       </c>
       <c r="B445" t="s">
-        <v>1157</v>
+        <v>936</v>
       </c>
       <c r="C445" t="s">
         <v>281</v>
       </c>
       <c r="D445">
-        <v>444</v>
+        <v>356</v>
       </c>
       <c r="E445" t="s">
-        <v>597</v>
+        <v>197</v>
       </c>
     </row>
     <row r="446" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
@@ -43758,7 +43758,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="450" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="450" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A450" t="s">
         <v>1166</v>
       </c>
@@ -44489,7 +44489,7 @@
         <v>1187</v>
       </c>
     </row>
-    <row r="493" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="493" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A493" t="s">
         <v>1272</v>
       </c>
@@ -44625,21 +44625,21 @@
         <v>1293</v>
       </c>
     </row>
-    <row r="501" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
+    <row r="501" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A501" t="s">
-        <v>1294</v>
+        <v>2145</v>
       </c>
       <c r="B501" t="s">
-        <v>1295</v>
+        <v>2146</v>
       </c>
       <c r="C501" t="s">
         <v>281</v>
       </c>
       <c r="D501">
-        <v>500</v>
+        <v>885</v>
       </c>
       <c r="E501" t="s">
-        <v>40</v>
+        <v>197</v>
       </c>
     </row>
     <row r="502" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
@@ -44710,7 +44710,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="506" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="506" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A506" t="s">
         <v>1306</v>
       </c>
@@ -44795,21 +44795,21 @@
         <v>197</v>
       </c>
     </row>
-    <row r="511" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
+    <row r="511" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A511" t="s">
-        <v>1316</v>
+        <v>952</v>
       </c>
       <c r="B511" t="s">
-        <v>1317</v>
+        <v>953</v>
       </c>
       <c r="C511" t="s">
         <v>281</v>
       </c>
       <c r="D511">
-        <v>510</v>
+        <v>363</v>
       </c>
       <c r="E511" t="s">
-        <v>66</v>
+        <v>717</v>
       </c>
     </row>
     <row r="512" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
@@ -44846,7 +44846,7 @@
         <v>905</v>
       </c>
     </row>
-    <row r="514" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="514" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A514" t="s">
         <v>1323</v>
       </c>
@@ -44965,21 +44965,21 @@
         <v>197</v>
       </c>
     </row>
-    <row r="521" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
+    <row r="521" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A521" t="s">
-        <v>1338</v>
+        <v>3636</v>
       </c>
       <c r="B521" t="s">
-        <v>1339</v>
+        <v>3637</v>
       </c>
       <c r="C521" t="s">
         <v>281</v>
       </c>
       <c r="D521">
-        <v>520</v>
+        <v>1587</v>
       </c>
       <c r="E521" t="s">
-        <v>711</v>
+        <v>717</v>
       </c>
     </row>
     <row r="522" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
@@ -45016,21 +45016,21 @@
         <v>484</v>
       </c>
     </row>
-    <row r="524" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
+    <row r="524" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A524" t="s">
-        <v>1345</v>
+        <v>2091</v>
       </c>
       <c r="B524" t="s">
-        <v>1346</v>
+        <v>2092</v>
       </c>
       <c r="C524" t="s">
         <v>281</v>
       </c>
       <c r="D524">
-        <v>523</v>
+        <v>859</v>
       </c>
       <c r="E524" t="s">
-        <v>1347</v>
+        <v>629</v>
       </c>
     </row>
     <row r="525" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
@@ -45101,21 +45101,21 @@
         <v>176</v>
       </c>
     </row>
-    <row r="529" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
+    <row r="529" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A529" t="s">
-        <v>1357</v>
+        <v>2525</v>
       </c>
       <c r="B529" t="s">
-        <v>1358</v>
+        <v>2526</v>
       </c>
       <c r="C529" t="s">
         <v>281</v>
       </c>
       <c r="D529">
-        <v>528</v>
+        <v>1062</v>
       </c>
       <c r="E529" t="s">
-        <v>708</v>
+        <v>629</v>
       </c>
     </row>
     <row r="530" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
@@ -45407,21 +45407,21 @@
         <v>650</v>
       </c>
     </row>
-    <row r="547" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
+    <row r="547" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A547" t="s">
-        <v>1395</v>
+        <v>3378</v>
       </c>
       <c r="B547" t="s">
-        <v>1396</v>
+        <v>3379</v>
       </c>
       <c r="C547" t="s">
         <v>281</v>
       </c>
       <c r="D547">
-        <v>546</v>
+        <v>1463</v>
       </c>
       <c r="E547" t="s">
-        <v>659</v>
+        <v>629</v>
       </c>
     </row>
     <row r="548" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
@@ -45458,21 +45458,21 @@
         <v>796</v>
       </c>
     </row>
-    <row r="550" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
+    <row r="550" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A550" t="s">
-        <v>1401</v>
+        <v>657</v>
       </c>
       <c r="B550" t="s">
-        <v>1402</v>
+        <v>658</v>
       </c>
       <c r="C550" t="s">
         <v>281</v>
       </c>
       <c r="D550">
-        <v>549</v>
+        <v>252</v>
       </c>
       <c r="E550" t="s">
-        <v>708</v>
+        <v>659</v>
       </c>
     </row>
     <row r="551" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
@@ -45679,21 +45679,21 @@
         <v>650</v>
       </c>
     </row>
-    <row r="563" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
+    <row r="563" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A563" t="s">
-        <v>1429</v>
+        <v>913</v>
       </c>
       <c r="B563" t="s">
-        <v>1430</v>
+        <v>914</v>
       </c>
       <c r="C563" t="s">
         <v>281</v>
       </c>
       <c r="D563">
-        <v>562</v>
+        <v>347</v>
       </c>
       <c r="E563" t="s">
-        <v>1431</v>
+        <v>659</v>
       </c>
     </row>
     <row r="564" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
@@ -46580,7 +46580,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="616" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="616" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A616" t="s">
         <v>1546</v>
       </c>
@@ -46801,7 +46801,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="629" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="629" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A629" t="s">
         <v>1575</v>
       </c>
@@ -47107,7 +47107,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="647" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="647" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A647" t="s">
         <v>1618</v>
       </c>
@@ -47549,7 +47549,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="673" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="673" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A673" t="s">
         <v>1679</v>
       </c>
@@ -48297,7 +48297,7 @@
         <v>668</v>
       </c>
     </row>
-    <row r="717" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="717" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A717" t="s">
         <v>1778</v>
       </c>
@@ -48586,21 +48586,21 @@
         <v>176</v>
       </c>
     </row>
-    <row r="734" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
+    <row r="734" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A734" t="s">
-        <v>1817</v>
+        <v>1395</v>
       </c>
       <c r="B734" t="s">
-        <v>1818</v>
+        <v>1396</v>
       </c>
       <c r="C734" t="s">
         <v>281</v>
       </c>
       <c r="D734">
-        <v>733</v>
+        <v>546</v>
       </c>
       <c r="E734" t="s">
-        <v>40</v>
+        <v>659</v>
       </c>
     </row>
     <row r="735" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
@@ -48671,72 +48671,72 @@
         <v>668</v>
       </c>
     </row>
-    <row r="739" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
+    <row r="739" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A739" t="s">
-        <v>1826</v>
+        <v>2089</v>
       </c>
       <c r="B739" t="s">
-        <v>1827</v>
+        <v>2090</v>
       </c>
       <c r="C739" t="s">
         <v>281</v>
       </c>
       <c r="D739">
-        <v>738</v>
+        <v>858</v>
       </c>
       <c r="E739" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="740" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
+        <v>659</v>
+      </c>
+    </row>
+    <row r="740" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A740" t="s">
-        <v>1828</v>
+        <v>4290</v>
       </c>
       <c r="B740" t="s">
-        <v>377</v>
+        <v>4291</v>
       </c>
       <c r="C740" t="s">
         <v>281</v>
       </c>
       <c r="D740">
-        <v>739</v>
+        <v>1898</v>
       </c>
       <c r="E740" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="741" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
+        <v>2109</v>
+      </c>
+    </row>
+    <row r="741" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A741" t="s">
-        <v>1829</v>
+        <v>376</v>
       </c>
       <c r="B741" t="s">
-        <v>1830</v>
+        <v>377</v>
       </c>
       <c r="C741" t="s">
         <v>281</v>
       </c>
       <c r="D741">
-        <v>740</v>
+        <v>140</v>
       </c>
       <c r="E741" t="s">
-        <v>484</v>
-      </c>
-    </row>
-    <row r="742" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="742" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A742" t="s">
-        <v>1831</v>
+        <v>386</v>
       </c>
       <c r="B742" t="s">
-        <v>1832</v>
+        <v>387</v>
       </c>
       <c r="C742" t="s">
         <v>281</v>
       </c>
       <c r="D742">
-        <v>741</v>
+        <v>144</v>
       </c>
       <c r="E742" t="s">
-        <v>701</v>
+        <v>176</v>
       </c>
     </row>
     <row r="743" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
@@ -48943,21 +48943,21 @@
         <v>66</v>
       </c>
     </row>
-    <row r="755" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
+    <row r="755" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A755" t="s">
-        <v>1859</v>
+        <v>551</v>
       </c>
       <c r="B755" t="s">
-        <v>1860</v>
+        <v>552</v>
       </c>
       <c r="C755" t="s">
         <v>281</v>
       </c>
       <c r="D755">
-        <v>754</v>
+        <v>211</v>
       </c>
       <c r="E755" t="s">
-        <v>711</v>
+        <v>176</v>
       </c>
     </row>
     <row r="756" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
@@ -48994,21 +48994,21 @@
         <v>40</v>
       </c>
     </row>
-    <row r="758" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
+    <row r="758" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A758" t="s">
-        <v>1865</v>
+        <v>893</v>
       </c>
       <c r="B758" t="s">
-        <v>1866</v>
+        <v>894</v>
       </c>
       <c r="C758" t="s">
         <v>281</v>
       </c>
       <c r="D758">
-        <v>757</v>
+        <v>339</v>
       </c>
       <c r="E758" t="s">
-        <v>838</v>
+        <v>176</v>
       </c>
     </row>
     <row r="759" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
@@ -49147,21 +49147,21 @@
         <v>796</v>
       </c>
     </row>
-    <row r="767" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
+    <row r="767" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A767" t="s">
-        <v>1884</v>
+        <v>1828</v>
       </c>
       <c r="B767" t="s">
-        <v>1885</v>
+        <v>377</v>
       </c>
       <c r="C767" t="s">
         <v>281</v>
       </c>
       <c r="D767">
-        <v>766</v>
+        <v>739</v>
       </c>
       <c r="E767" t="s">
-        <v>610</v>
+        <v>176</v>
       </c>
     </row>
     <row r="768" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
@@ -49215,21 +49215,21 @@
         <v>600</v>
       </c>
     </row>
-    <row r="771" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
+    <row r="771" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A771" t="s">
-        <v>1892</v>
+        <v>1916</v>
       </c>
       <c r="B771" t="s">
-        <v>1893</v>
+        <v>1917</v>
       </c>
       <c r="C771" t="s">
         <v>281</v>
       </c>
       <c r="D771">
-        <v>770</v>
+        <v>779</v>
       </c>
       <c r="E771" t="s">
-        <v>1894</v>
+        <v>176</v>
       </c>
     </row>
     <row r="772" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
@@ -49368,18 +49368,18 @@
         <v>40</v>
       </c>
     </row>
-    <row r="780" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
+    <row r="780" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A780" t="s">
-        <v>1916</v>
+        <v>2149</v>
       </c>
       <c r="B780" t="s">
-        <v>1917</v>
+        <v>2150</v>
       </c>
       <c r="C780" t="s">
         <v>281</v>
       </c>
       <c r="D780">
-        <v>779</v>
+        <v>887</v>
       </c>
       <c r="E780" t="s">
         <v>176</v>
@@ -49419,21 +49419,21 @@
         <v>89</v>
       </c>
     </row>
-    <row r="783" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
+    <row r="783" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A783" t="s">
-        <v>1923</v>
+        <v>2440</v>
       </c>
       <c r="B783" t="s">
-        <v>1924</v>
+        <v>2441</v>
       </c>
       <c r="C783" t="s">
         <v>281</v>
       </c>
       <c r="D783">
-        <v>782</v>
+        <v>1020</v>
       </c>
       <c r="E783" t="s">
-        <v>66</v>
+        <v>176</v>
       </c>
     </row>
     <row r="784" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
@@ -49521,21 +49521,21 @@
         <v>40</v>
       </c>
     </row>
-    <row r="789" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
+    <row r="789" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A789" t="s">
-        <v>1936</v>
+        <v>2521</v>
       </c>
       <c r="B789" t="s">
-        <v>1937</v>
+        <v>2522</v>
       </c>
       <c r="C789" t="s">
         <v>281</v>
       </c>
       <c r="D789">
-        <v>788</v>
+        <v>1060</v>
       </c>
       <c r="E789" t="s">
-        <v>668</v>
+        <v>866</v>
       </c>
     </row>
     <row r="790" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
@@ -49623,21 +49623,21 @@
         <v>66</v>
       </c>
     </row>
-    <row r="795" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
+    <row r="795" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A795" t="s">
-        <v>1949</v>
+        <v>1865</v>
       </c>
       <c r="B795" t="s">
-        <v>1950</v>
+        <v>1866</v>
       </c>
       <c r="C795" t="s">
         <v>281</v>
       </c>
       <c r="D795">
-        <v>794</v>
+        <v>757</v>
       </c>
       <c r="E795" t="s">
-        <v>600</v>
+        <v>838</v>
       </c>
     </row>
     <row r="796" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
@@ -49759,21 +49759,21 @@
         <v>66</v>
       </c>
     </row>
-    <row r="803" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
+    <row r="803" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A803" t="s">
-        <v>1965</v>
+        <v>3469</v>
       </c>
       <c r="B803" t="s">
-        <v>1966</v>
+        <v>3470</v>
       </c>
       <c r="C803" t="s">
         <v>281</v>
       </c>
       <c r="D803">
-        <v>802</v>
+        <v>1507</v>
       </c>
       <c r="E803" t="s">
-        <v>1967</v>
+        <v>838</v>
       </c>
     </row>
     <row r="804" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
@@ -49980,7 +49980,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="816" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="816" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A816" t="s">
         <v>2000</v>
       </c>
@@ -50371,21 +50371,21 @@
         <v>40</v>
       </c>
     </row>
-    <row r="839" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
+    <row r="839" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A839" t="s">
-        <v>2050</v>
+        <v>4180</v>
       </c>
       <c r="B839" t="s">
-        <v>2051</v>
+        <v>1866</v>
       </c>
       <c r="C839" t="s">
         <v>281</v>
       </c>
       <c r="D839">
+        <v>1845</v>
+      </c>
+      <c r="E839" t="s">
         <v>838</v>
-      </c>
-      <c r="E839" t="s">
-        <v>938</v>
       </c>
     </row>
     <row r="840" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
@@ -50422,7 +50422,7 @@
         <v>763</v>
       </c>
     </row>
-    <row r="842" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="842" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A842" t="s">
         <v>2056</v>
       </c>
@@ -50643,21 +50643,21 @@
         <v>629</v>
       </c>
     </row>
-    <row r="855" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
+    <row r="855" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A855" t="s">
-        <v>2082</v>
+        <v>315</v>
       </c>
       <c r="B855" t="s">
-        <v>2083</v>
+        <v>316</v>
       </c>
       <c r="C855" t="s">
         <v>281</v>
       </c>
       <c r="D855">
-        <v>854</v>
+        <v>114</v>
       </c>
       <c r="E855" t="s">
-        <v>66</v>
+        <v>89</v>
       </c>
     </row>
     <row r="856" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
@@ -50694,89 +50694,89 @@
         <v>122</v>
       </c>
     </row>
-    <row r="858" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
+    <row r="858" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A858" t="s">
-        <v>2087</v>
+        <v>406</v>
       </c>
       <c r="B858" t="s">
-        <v>2088</v>
+        <v>407</v>
       </c>
       <c r="C858" t="s">
         <v>281</v>
       </c>
       <c r="D858">
-        <v>857</v>
+        <v>152</v>
       </c>
       <c r="E858" t="s">
-        <v>967</v>
-      </c>
-    </row>
-    <row r="859" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="859" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A859" t="s">
-        <v>2089</v>
+        <v>885</v>
       </c>
       <c r="B859" t="s">
-        <v>2090</v>
+        <v>886</v>
       </c>
       <c r="C859" t="s">
         <v>281</v>
       </c>
       <c r="D859">
-        <v>858</v>
+        <v>336</v>
       </c>
       <c r="E859" t="s">
-        <v>659</v>
-      </c>
-    </row>
-    <row r="860" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
+        <v>701</v>
+      </c>
+    </row>
+    <row r="860" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A860" t="s">
-        <v>2091</v>
+        <v>1831</v>
       </c>
       <c r="B860" t="s">
-        <v>2092</v>
+        <v>1832</v>
       </c>
       <c r="C860" t="s">
         <v>281</v>
       </c>
       <c r="D860">
-        <v>859</v>
+        <v>741</v>
       </c>
       <c r="E860" t="s">
-        <v>629</v>
-      </c>
-    </row>
-    <row r="861" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
+        <v>701</v>
+      </c>
+    </row>
+    <row r="861" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A861" t="s">
-        <v>2093</v>
+        <v>625</v>
       </c>
       <c r="B861" t="s">
-        <v>2094</v>
+        <v>626</v>
       </c>
       <c r="C861" t="s">
         <v>281</v>
       </c>
       <c r="D861">
-        <v>860</v>
+        <v>240</v>
       </c>
       <c r="E861" t="s">
-        <v>977</v>
-      </c>
-    </row>
-    <row r="862" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="862" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A862" t="s">
-        <v>2095</v>
+        <v>792</v>
       </c>
       <c r="B862" t="s">
-        <v>2096</v>
+        <v>793</v>
       </c>
       <c r="C862" t="s">
         <v>281</v>
       </c>
       <c r="D862">
-        <v>861</v>
+        <v>299</v>
       </c>
       <c r="E862" t="s">
-        <v>961</v>
+        <v>597</v>
       </c>
     </row>
     <row r="863" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
@@ -51034,7 +51034,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="878" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="878" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A878" t="s">
         <v>2129</v>
       </c>
@@ -51119,7 +51119,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="883" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="883" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A883" t="s">
         <v>2139</v>
       </c>
@@ -51170,72 +51170,72 @@
         <v>1078</v>
       </c>
     </row>
-    <row r="886" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
+    <row r="886" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A886" t="s">
-        <v>2145</v>
+        <v>1156</v>
       </c>
       <c r="B886" t="s">
-        <v>2146</v>
+        <v>1157</v>
       </c>
       <c r="C886" t="s">
         <v>281</v>
       </c>
       <c r="D886">
-        <v>885</v>
+        <v>444</v>
       </c>
       <c r="E886" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="887" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="887" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A887" t="s">
-        <v>2147</v>
+        <v>588</v>
       </c>
       <c r="B887" t="s">
-        <v>2148</v>
+        <v>589</v>
       </c>
       <c r="C887" t="s">
         <v>281</v>
       </c>
       <c r="D887">
-        <v>886</v>
+        <v>226</v>
       </c>
       <c r="E887" t="s">
-        <v>600</v>
-      </c>
-    </row>
-    <row r="888" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
+        <v>590</v>
+      </c>
+    </row>
+    <row r="888" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A888" t="s">
-        <v>2149</v>
+        <v>4946</v>
       </c>
       <c r="B888" t="s">
-        <v>2150</v>
+        <v>4947</v>
       </c>
       <c r="C888" t="s">
         <v>281</v>
       </c>
       <c r="D888">
-        <v>887</v>
+        <v>2210</v>
       </c>
       <c r="E888" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="889" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
+        <v>4701</v>
+      </c>
+    </row>
+    <row r="889" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A889" t="s">
-        <v>2151</v>
+        <v>806</v>
       </c>
       <c r="B889" t="s">
-        <v>2152</v>
+        <v>807</v>
       </c>
       <c r="C889" t="s">
         <v>281</v>
       </c>
       <c r="D889">
-        <v>888</v>
+        <v>305</v>
       </c>
       <c r="E889" t="s">
-        <v>708</v>
+        <v>808</v>
       </c>
     </row>
     <row r="890" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
@@ -51255,7 +51255,7 @@
         <v>796</v>
       </c>
     </row>
-    <row r="891" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="891" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A891" t="s">
         <v>2156</v>
       </c>
@@ -51272,21 +51272,21 @@
         <v>176</v>
       </c>
     </row>
-    <row r="892" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
+    <row r="892" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A892" t="s">
-        <v>2158</v>
+        <v>825</v>
       </c>
       <c r="B892" t="s">
-        <v>2159</v>
+        <v>826</v>
       </c>
       <c r="C892" t="s">
         <v>281</v>
       </c>
       <c r="D892">
-        <v>891</v>
+        <v>312</v>
       </c>
       <c r="E892" t="s">
-        <v>720</v>
+        <v>808</v>
       </c>
     </row>
     <row r="893" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
@@ -51391,7 +51391,7 @@
         <v>763</v>
       </c>
     </row>
-    <row r="899" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="899" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A899" t="s">
         <v>2173</v>
       </c>
@@ -51493,21 +51493,21 @@
         <v>866</v>
       </c>
     </row>
-    <row r="905" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
+    <row r="905" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A905" t="s">
-        <v>2186</v>
+        <v>319</v>
       </c>
       <c r="B905" t="s">
-        <v>2187</v>
+        <v>320</v>
       </c>
       <c r="C905" t="s">
         <v>281</v>
       </c>
       <c r="D905">
-        <v>904</v>
+        <v>116</v>
       </c>
       <c r="E905" t="s">
-        <v>708</v>
+        <v>7</v>
       </c>
     </row>
     <row r="906" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
@@ -51646,7 +51646,7 @@
         <v>618</v>
       </c>
     </row>
-    <row r="914" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="914" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A914" t="s">
         <v>2208</v>
       </c>
@@ -51680,7 +51680,7 @@
         <v>1009</v>
       </c>
     </row>
-    <row r="916" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="916" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A916" t="s">
         <v>2212</v>
       </c>
@@ -53312,7 +53312,7 @@
         <v>678</v>
       </c>
     </row>
-    <row r="1012" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="1012" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A1012" t="s">
         <v>2420</v>
       </c>
@@ -53465,21 +53465,21 @@
         <v>711</v>
       </c>
     </row>
-    <row r="1021" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
+    <row r="1021" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A1021" t="s">
-        <v>2440</v>
+        <v>4111</v>
       </c>
       <c r="B1021" t="s">
-        <v>2441</v>
+        <v>4112</v>
       </c>
       <c r="C1021" t="s">
         <v>281</v>
       </c>
       <c r="D1021">
-        <v>1020</v>
+        <v>1810</v>
       </c>
       <c r="E1021" t="s">
-        <v>176</v>
+        <v>7</v>
       </c>
     </row>
     <row r="1022" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
@@ -53550,21 +53550,21 @@
         <v>659</v>
       </c>
     </row>
-    <row r="1026" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
+    <row r="1026" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A1026" t="s">
-        <v>2450</v>
+        <v>801</v>
       </c>
       <c r="B1026" t="s">
-        <v>2451</v>
+        <v>802</v>
       </c>
       <c r="C1026" t="s">
         <v>281</v>
       </c>
       <c r="D1026">
-        <v>1025</v>
+        <v>303</v>
       </c>
       <c r="E1026" t="s">
-        <v>1347</v>
+        <v>247</v>
       </c>
     </row>
     <row r="1027" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
@@ -54145,21 +54145,21 @@
         <v>866</v>
       </c>
     </row>
-    <row r="1061" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
+    <row r="1061" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A1061" t="s">
-        <v>2521</v>
+        <v>881</v>
       </c>
       <c r="B1061" t="s">
-        <v>2522</v>
+        <v>882</v>
       </c>
       <c r="C1061" t="s">
         <v>281</v>
       </c>
       <c r="D1061">
-        <v>1060</v>
+        <v>334</v>
       </c>
       <c r="E1061" t="s">
-        <v>866</v>
+        <v>247</v>
       </c>
     </row>
     <row r="1062" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
@@ -54179,55 +54179,55 @@
         <v>1078</v>
       </c>
     </row>
-    <row r="1063" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
+    <row r="1063" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A1063" t="s">
-        <v>2525</v>
+        <v>799</v>
       </c>
       <c r="B1063" t="s">
-        <v>2526</v>
+        <v>800</v>
       </c>
       <c r="C1063" t="s">
         <v>281</v>
       </c>
       <c r="D1063">
-        <v>1062</v>
+        <v>302</v>
       </c>
       <c r="E1063" t="s">
-        <v>629</v>
-      </c>
-    </row>
-    <row r="1064" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
+        <v>678</v>
+      </c>
+    </row>
+    <row r="1064" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A1064" t="s">
-        <v>2527</v>
+        <v>2050</v>
       </c>
       <c r="B1064" t="s">
-        <v>2528</v>
+        <v>2051</v>
       </c>
       <c r="C1064" t="s">
         <v>281</v>
       </c>
       <c r="D1064">
-        <v>1063</v>
+        <v>838</v>
       </c>
       <c r="E1064" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="1065" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
+        <v>938</v>
+      </c>
+    </row>
+    <row r="1065" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A1065" t="s">
-        <v>2529</v>
+        <v>585</v>
       </c>
       <c r="B1065" t="s">
-        <v>2530</v>
+        <v>586</v>
       </c>
       <c r="C1065" t="s">
         <v>281</v>
       </c>
       <c r="D1065">
-        <v>1064</v>
+        <v>225</v>
       </c>
       <c r="E1065" t="s">
-        <v>920</v>
+        <v>587</v>
       </c>
     </row>
     <row r="1066" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
@@ -54315,21 +54315,21 @@
         <v>838</v>
       </c>
     </row>
-    <row r="1071" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
+    <row r="1071" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A1071" t="s">
-        <v>2542</v>
+        <v>593</v>
       </c>
       <c r="B1071" t="s">
-        <v>2543</v>
+        <v>594</v>
       </c>
       <c r="C1071" t="s">
         <v>281</v>
       </c>
       <c r="D1071">
-        <v>1070</v>
+        <v>228</v>
       </c>
       <c r="E1071" t="s">
-        <v>720</v>
+        <v>587</v>
       </c>
     </row>
     <row r="1072" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
@@ -54366,21 +54366,21 @@
         <v>66</v>
       </c>
     </row>
-    <row r="1074" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
+    <row r="1074" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A1074" t="s">
-        <v>2548</v>
+        <v>3534</v>
       </c>
       <c r="B1074" t="s">
-        <v>2549</v>
+        <v>3535</v>
       </c>
       <c r="C1074" t="s">
         <v>281</v>
       </c>
       <c r="D1074">
-        <v>1073</v>
+        <v>1539</v>
       </c>
       <c r="E1074" t="s">
-        <v>791</v>
+        <v>587</v>
       </c>
     </row>
     <row r="1075" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
@@ -54604,21 +54604,21 @@
         <v>600</v>
       </c>
     </row>
-    <row r="1088" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
+    <row r="1088" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A1088" t="s">
-        <v>2577</v>
+        <v>660</v>
       </c>
       <c r="B1088" t="s">
-        <v>2578</v>
+        <v>661</v>
       </c>
       <c r="C1088" t="s">
         <v>281</v>
       </c>
       <c r="D1088">
-        <v>1087</v>
+        <v>253</v>
       </c>
       <c r="E1088" t="s">
-        <v>986</v>
+        <v>662</v>
       </c>
     </row>
     <row r="1089" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
@@ -55284,7 +55284,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="1128" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="1128" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A1128" t="s">
         <v>2667</v>
       </c>
@@ -55590,7 +55590,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="1146" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="1146" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A1146" t="s">
         <v>2706</v>
       </c>
@@ -55709,7 +55709,7 @@
         <v>1114</v>
       </c>
     </row>
-    <row r="1153" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="1153" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A1153" t="s">
         <v>2721</v>
       </c>
@@ -55726,7 +55726,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="1154" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="1154" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A1154" t="s">
         <v>2723</v>
       </c>
@@ -55896,7 +55896,7 @@
         <v>650</v>
       </c>
     </row>
-    <row r="1164" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="1164" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A1164" t="s">
         <v>2743</v>
       </c>
@@ -56678,7 +56678,7 @@
         <v>720</v>
       </c>
     </row>
-    <row r="1210" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="1210" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A1210" t="s">
         <v>2842</v>
       </c>
@@ -57052,7 +57052,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="1232" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="1232" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A1232" t="s">
         <v>2891</v>
       </c>
@@ -57239,7 +57239,7 @@
         <v>1078</v>
       </c>
     </row>
-    <row r="1243" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="1243" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A1243" t="s">
         <v>2914</v>
       </c>
@@ -57443,7 +57443,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="1255" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="1255" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A1255" t="s">
         <v>2939</v>
       </c>
@@ -57460,7 +57460,7 @@
         <v>640</v>
       </c>
     </row>
-    <row r="1256" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="1256" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A1256" t="s">
         <v>2941</v>
       </c>
@@ -57528,7 +57528,7 @@
         <v>708</v>
       </c>
     </row>
-    <row r="1260" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="1260" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A1260" t="s">
         <v>2949</v>
       </c>
@@ -57562,7 +57562,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="1262" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="1262" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A1262" t="s">
         <v>2953</v>
       </c>
@@ -57579,7 +57579,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="1263" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="1263" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A1263" t="s">
         <v>2955</v>
       </c>
@@ -57766,7 +57766,7 @@
         <v>763</v>
       </c>
     </row>
-    <row r="1274" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="1274" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A1274" t="s">
         <v>2978</v>
       </c>
@@ -58276,18 +58276,18 @@
         <v>40</v>
       </c>
     </row>
-    <row r="1304" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
+    <row r="1304" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A1304" t="s">
-        <v>3038</v>
+        <v>323</v>
       </c>
       <c r="B1304" t="s">
-        <v>3039</v>
+        <v>324</v>
       </c>
       <c r="C1304" t="s">
         <v>281</v>
       </c>
       <c r="D1304">
-        <v>1303</v>
+        <v>118</v>
       </c>
       <c r="E1304" t="s">
         <v>47</v>
@@ -58514,38 +58514,38 @@
         <v>650</v>
       </c>
     </row>
-    <row r="1318" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
+    <row r="1318" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A1318" t="s">
-        <v>3066</v>
+        <v>327</v>
       </c>
       <c r="B1318" t="s">
-        <v>3067</v>
+        <v>328</v>
       </c>
       <c r="C1318" t="s">
         <v>281</v>
       </c>
       <c r="D1318">
-        <v>1317</v>
+        <v>120</v>
       </c>
       <c r="E1318" t="s">
-        <v>796</v>
-      </c>
-    </row>
-    <row r="1319" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="1319" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A1319" t="s">
-        <v>3068</v>
+        <v>352</v>
       </c>
       <c r="B1319" t="s">
-        <v>3069</v>
+        <v>353</v>
       </c>
       <c r="C1319" t="s">
         <v>281</v>
       </c>
       <c r="D1319">
-        <v>1318</v>
+        <v>130</v>
       </c>
       <c r="E1319" t="s">
-        <v>1078</v>
+        <v>47</v>
       </c>
     </row>
     <row r="1320" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
@@ -58854,38 +58854,38 @@
         <v>796</v>
       </c>
     </row>
-    <row r="1338" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
+    <row r="1338" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A1338" t="s">
-        <v>3109</v>
+        <v>3038</v>
       </c>
       <c r="B1338" t="s">
-        <v>3110</v>
+        <v>3039</v>
       </c>
       <c r="C1338" t="s">
         <v>281</v>
       </c>
       <c r="D1338">
-        <v>1337</v>
+        <v>1303</v>
       </c>
       <c r="E1338" t="s">
-        <v>832</v>
-      </c>
-    </row>
-    <row r="1339" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="1339" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A1339" t="s">
-        <v>3111</v>
+        <v>4129</v>
       </c>
       <c r="B1339" t="s">
-        <v>3112</v>
+        <v>4130</v>
       </c>
       <c r="C1339" t="s">
         <v>281</v>
       </c>
       <c r="D1339">
-        <v>1338</v>
+        <v>1819</v>
       </c>
       <c r="E1339" t="s">
-        <v>832</v>
+        <v>47</v>
       </c>
     </row>
     <row r="1340" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
@@ -58990,7 +58990,7 @@
         <v>708</v>
       </c>
     </row>
-    <row r="1346" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="1346" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A1346" t="s">
         <v>3125</v>
       </c>
@@ -60401,7 +60401,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="1429" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="1429" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A1429" t="s">
         <v>3307</v>
       </c>
@@ -60486,7 +60486,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="1434" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="1434" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A1434" t="s">
         <v>3318</v>
       </c>
@@ -60690,7 +60690,7 @@
         <v>678</v>
       </c>
     </row>
-    <row r="1446" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="1446" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A1446" t="s">
         <v>3341</v>
       </c>
@@ -60860,21 +60860,21 @@
         <v>484</v>
       </c>
     </row>
-    <row r="1456" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
+    <row r="1456" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A1456" t="s">
-        <v>3362</v>
+        <v>794</v>
       </c>
       <c r="B1456" t="s">
-        <v>3363</v>
+        <v>795</v>
       </c>
       <c r="C1456" t="s">
         <v>281</v>
       </c>
       <c r="D1456">
-        <v>1455</v>
+        <v>300</v>
       </c>
       <c r="E1456" t="s">
-        <v>66</v>
+        <v>796</v>
       </c>
     </row>
     <row r="1457" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
@@ -60996,21 +60996,21 @@
         <v>645</v>
       </c>
     </row>
-    <row r="1464" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
+    <row r="1464" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A1464" t="s">
-        <v>3378</v>
+        <v>3066</v>
       </c>
       <c r="B1464" t="s">
-        <v>3379</v>
+        <v>3067</v>
       </c>
       <c r="C1464" t="s">
         <v>281</v>
       </c>
       <c r="D1464">
-        <v>1463</v>
+        <v>1317</v>
       </c>
       <c r="E1464" t="s">
-        <v>629</v>
+        <v>796</v>
       </c>
     </row>
     <row r="1465" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
@@ -61659,7 +61659,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="1503" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="1503" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A1503" t="s">
         <v>3458</v>
       </c>
@@ -61744,21 +61744,21 @@
         <v>796</v>
       </c>
     </row>
-    <row r="1508" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
+    <row r="1508" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A1508" t="s">
-        <v>3469</v>
+        <v>2158</v>
       </c>
       <c r="B1508" t="s">
-        <v>3470</v>
+        <v>2159</v>
       </c>
       <c r="C1508" t="s">
         <v>281</v>
       </c>
       <c r="D1508">
-        <v>1507</v>
+        <v>891</v>
       </c>
       <c r="E1508" t="s">
-        <v>838</v>
+        <v>720</v>
       </c>
     </row>
     <row r="1509" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
@@ -62016,7 +62016,7 @@
         <v>668</v>
       </c>
     </row>
-    <row r="1524" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="1524" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A1524" t="s">
         <v>3501</v>
       </c>
@@ -62084,7 +62084,7 @@
         <v>668</v>
       </c>
     </row>
-    <row r="1528" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="1528" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A1528" t="s">
         <v>3509</v>
       </c>
@@ -62135,21 +62135,21 @@
         <v>678</v>
       </c>
     </row>
-    <row r="1531" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
+    <row r="1531" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A1531" t="s">
-        <v>3515</v>
+        <v>2542</v>
       </c>
       <c r="B1531" t="s">
-        <v>3516</v>
+        <v>2543</v>
       </c>
       <c r="C1531" t="s">
         <v>281</v>
       </c>
       <c r="D1531">
-        <v>1530</v>
+        <v>1070</v>
       </c>
       <c r="E1531" t="s">
-        <v>1003</v>
+        <v>720</v>
       </c>
     </row>
     <row r="1532" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
@@ -62288,38 +62288,38 @@
         <v>590</v>
       </c>
     </row>
-    <row r="1540" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
+    <row r="1540" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A1540" t="s">
-        <v>3534</v>
+        <v>959</v>
       </c>
       <c r="B1540" t="s">
-        <v>3535</v>
+        <v>960</v>
       </c>
       <c r="C1540" t="s">
         <v>281</v>
       </c>
       <c r="D1540">
-        <v>1539</v>
+        <v>366</v>
       </c>
       <c r="E1540" t="s">
-        <v>587</v>
-      </c>
-    </row>
-    <row r="1541" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
+        <v>961</v>
+      </c>
+    </row>
+    <row r="1541" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A1541" t="s">
-        <v>3536</v>
+        <v>2095</v>
       </c>
       <c r="B1541" t="s">
-        <v>3537</v>
+        <v>2096</v>
       </c>
       <c r="C1541" t="s">
         <v>281</v>
       </c>
       <c r="D1541">
-        <v>1540</v>
+        <v>861</v>
       </c>
       <c r="E1541" t="s">
-        <v>618</v>
+        <v>961</v>
       </c>
     </row>
     <row r="1542" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
@@ -62441,7 +62441,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="1549" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="1549" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A1549" t="s">
         <v>3554</v>
       </c>
@@ -62560,7 +62560,7 @@
         <v>977</v>
       </c>
     </row>
-    <row r="1556" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="1556" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A1556" t="s">
         <v>3568</v>
       </c>
@@ -62764,7 +62764,7 @@
         <v>708</v>
       </c>
     </row>
-    <row r="1568" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="1568" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A1568" t="s">
         <v>3593</v>
       </c>
@@ -62798,7 +62798,7 @@
         <v>606</v>
       </c>
     </row>
-    <row r="1570" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="1570" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A1570" t="s">
         <v>3597</v>
       </c>
@@ -62985,7 +62985,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="1581" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="1581" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A1581" t="s">
         <v>3623</v>
       </c>
@@ -63087,38 +63087,38 @@
         <v>484</v>
       </c>
     </row>
-    <row r="1587" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
+    <row r="1587" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A1587" t="s">
-        <v>3634</v>
+        <v>3640</v>
       </c>
       <c r="B1587" t="s">
-        <v>3635</v>
+        <v>3641</v>
       </c>
       <c r="C1587" t="s">
         <v>281</v>
       </c>
       <c r="D1587">
-        <v>1586</v>
+        <v>1589</v>
       </c>
       <c r="E1587" t="s">
-        <v>650</v>
-      </c>
-    </row>
-    <row r="1588" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
+        <v>961</v>
+      </c>
+    </row>
+    <row r="1588" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A1588" t="s">
-        <v>3636</v>
+        <v>2577</v>
       </c>
       <c r="B1588" t="s">
-        <v>3637</v>
+        <v>2578</v>
       </c>
       <c r="C1588" t="s">
         <v>281</v>
       </c>
       <c r="D1588">
-        <v>1587</v>
+        <v>1087</v>
       </c>
       <c r="E1588" t="s">
-        <v>717</v>
+        <v>986</v>
       </c>
     </row>
     <row r="1589" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
@@ -63138,21 +63138,21 @@
         <v>763</v>
       </c>
     </row>
-    <row r="1590" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
+    <row r="1590" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A1590" t="s">
-        <v>3640</v>
+        <v>4189</v>
       </c>
       <c r="B1590" t="s">
-        <v>3641</v>
+        <v>4190</v>
       </c>
       <c r="C1590" t="s">
         <v>281</v>
       </c>
       <c r="D1590">
-        <v>1589</v>
+        <v>1850</v>
       </c>
       <c r="E1590" t="s">
-        <v>961</v>
+        <v>986</v>
       </c>
     </row>
     <row r="1591" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
@@ -64056,7 +64056,7 @@
         <v>1114</v>
       </c>
     </row>
-    <row r="1644" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="1644" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A1644" t="s">
         <v>3758</v>
       </c>
@@ -64243,7 +64243,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="1655" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="1655" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A1655" t="s">
         <v>3781</v>
       </c>
@@ -64260,7 +64260,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="1656" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="1656" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A1656" t="s">
         <v>3783</v>
       </c>
@@ -64583,21 +64583,21 @@
         <v>484</v>
       </c>
     </row>
-    <row r="1675" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
+    <row r="1675" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A1675" t="s">
-        <v>3821</v>
+        <v>4208</v>
       </c>
       <c r="B1675" t="s">
-        <v>3822</v>
+        <v>4209</v>
       </c>
       <c r="C1675" t="s">
         <v>281</v>
       </c>
       <c r="D1675">
-        <v>1674</v>
+        <v>1859</v>
       </c>
       <c r="E1675" t="s">
-        <v>600</v>
+        <v>3900</v>
       </c>
     </row>
     <row r="1676" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
@@ -64821,7 +64821,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="1689" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="1689" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A1689" t="s">
         <v>3852</v>
       </c>
@@ -65331,21 +65331,21 @@
         <v>40</v>
       </c>
     </row>
-    <row r="1719" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
+    <row r="1719" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A1719" t="s">
-        <v>3919</v>
+        <v>1892</v>
       </c>
       <c r="B1719" t="s">
-        <v>3920</v>
+        <v>1893</v>
       </c>
       <c r="C1719" t="s">
         <v>281</v>
       </c>
       <c r="D1719">
-        <v>1718</v>
+        <v>770</v>
       </c>
       <c r="E1719" t="s">
-        <v>600</v>
+        <v>1894</v>
       </c>
     </row>
     <row r="1720" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
@@ -65467,7 +65467,7 @@
         <v>791</v>
       </c>
     </row>
-    <row r="1727" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="1727" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A1727" t="s">
         <v>3935</v>
       </c>
@@ -65586,21 +65586,21 @@
         <v>2316</v>
       </c>
     </row>
-    <row r="1734" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
+    <row r="1734" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A1734" t="s">
-        <v>3950</v>
+        <v>450</v>
       </c>
       <c r="B1734" t="s">
-        <v>3951</v>
+        <v>451</v>
       </c>
       <c r="C1734" t="s">
         <v>281</v>
       </c>
       <c r="D1734">
-        <v>1733</v>
+        <v>170</v>
       </c>
       <c r="E1734" t="s">
-        <v>576</v>
+        <v>122</v>
       </c>
     </row>
     <row r="1735" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
@@ -66011,7 +66011,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="1759" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="1759" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A1759" t="s">
         <v>4005</v>
       </c>
@@ -66368,21 +66368,21 @@
         <v>7</v>
       </c>
     </row>
-    <row r="1780" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
+    <row r="1780" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A1780" t="s">
-        <v>4048</v>
+        <v>648</v>
       </c>
       <c r="B1780" t="s">
-        <v>4049</v>
+        <v>649</v>
       </c>
       <c r="C1780" t="s">
         <v>281</v>
       </c>
       <c r="D1780">
-        <v>1779</v>
+        <v>249</v>
       </c>
       <c r="E1780" t="s">
-        <v>66</v>
+        <v>650</v>
       </c>
     </row>
     <row r="1781" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
@@ -66538,21 +66538,21 @@
         <v>1009</v>
       </c>
     </row>
-    <row r="1790" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
+    <row r="1790" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A1790" t="s">
-        <v>4069</v>
+        <v>3634</v>
       </c>
       <c r="B1790" t="s">
-        <v>4070</v>
+        <v>3635</v>
       </c>
       <c r="C1790" t="s">
         <v>281</v>
       </c>
       <c r="D1790">
-        <v>1789</v>
+        <v>1586</v>
       </c>
       <c r="E1790" t="s">
-        <v>618</v>
+        <v>650</v>
       </c>
     </row>
     <row r="1791" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
@@ -66572,21 +66572,21 @@
         <v>66</v>
       </c>
     </row>
-    <row r="1792" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
+    <row r="1792" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A1792" t="s">
-        <v>4073</v>
+        <v>4822</v>
       </c>
       <c r="B1792" t="s">
-        <v>4074</v>
+        <v>4823</v>
       </c>
       <c r="C1792" t="s">
         <v>281</v>
       </c>
       <c r="D1792">
-        <v>1791</v>
+        <v>2151</v>
       </c>
       <c r="E1792" t="s">
-        <v>708</v>
+        <v>650</v>
       </c>
     </row>
     <row r="1793" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
@@ -66793,7 +66793,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="1805" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="1805" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A1805" t="s">
         <v>4099</v>
       </c>
@@ -66827,7 +66827,7 @@
         <v>1146</v>
       </c>
     </row>
-    <row r="1807" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="1807" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A1807" t="s">
         <v>4103</v>
       </c>
@@ -66895,21 +66895,21 @@
         <v>659</v>
       </c>
     </row>
-    <row r="1811" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
+    <row r="1811" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A1811" t="s">
-        <v>4111</v>
+        <v>1949</v>
       </c>
       <c r="B1811" t="s">
-        <v>4112</v>
+        <v>1950</v>
       </c>
       <c r="C1811" t="s">
         <v>281</v>
       </c>
       <c r="D1811">
-        <v>1810</v>
+        <v>794</v>
       </c>
       <c r="E1811" t="s">
-        <v>7</v>
+        <v>600</v>
       </c>
     </row>
     <row r="1812" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
@@ -67048,21 +67048,21 @@
         <v>47</v>
       </c>
     </row>
-    <row r="1820" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
+    <row r="1820" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A1820" t="s">
-        <v>4129</v>
+        <v>2147</v>
       </c>
       <c r="B1820" t="s">
-        <v>4130</v>
+        <v>2148</v>
       </c>
       <c r="C1820" t="s">
         <v>281</v>
       </c>
       <c r="D1820">
-        <v>1819</v>
+        <v>886</v>
       </c>
       <c r="E1820" t="s">
-        <v>47</v>
+        <v>600</v>
       </c>
     </row>
     <row r="1821" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
@@ -67099,7 +67099,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="1823" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="1823" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A1823" t="s">
         <v>4135</v>
       </c>
@@ -67116,38 +67116,38 @@
         <v>197</v>
       </c>
     </row>
-    <row r="1824" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
+    <row r="1824" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A1824" t="s">
-        <v>4137</v>
+        <v>3821</v>
       </c>
       <c r="B1824" t="s">
-        <v>4138</v>
+        <v>3822</v>
       </c>
       <c r="C1824" t="s">
         <v>281</v>
       </c>
       <c r="D1824">
-        <v>1823</v>
+        <v>1674</v>
       </c>
       <c r="E1824" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="1825" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="1825" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A1825" t="s">
-        <v>4139</v>
+        <v>3919</v>
       </c>
       <c r="B1825" t="s">
-        <v>4140</v>
+        <v>3920</v>
       </c>
       <c r="C1825" t="s">
         <v>281</v>
       </c>
       <c r="D1825">
-        <v>1824</v>
+        <v>1718</v>
       </c>
       <c r="E1825" t="s">
-        <v>66</v>
+        <v>600</v>
       </c>
     </row>
     <row r="1826" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
@@ -67269,21 +67269,21 @@
         <v>645</v>
       </c>
     </row>
-    <row r="1833" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
+    <row r="1833" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A1833" t="s">
-        <v>4155</v>
+        <v>1345</v>
       </c>
       <c r="B1833" t="s">
-        <v>4156</v>
+        <v>1346</v>
       </c>
       <c r="C1833" t="s">
         <v>281</v>
       </c>
       <c r="D1833">
-        <v>1832</v>
+        <v>523</v>
       </c>
       <c r="E1833" t="s">
-        <v>832</v>
+        <v>1347</v>
       </c>
     </row>
     <row r="1834" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
@@ -67490,21 +67490,21 @@
         <v>701</v>
       </c>
     </row>
-    <row r="1846" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
+    <row r="1846" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A1846" t="s">
-        <v>4180</v>
+        <v>2450</v>
       </c>
       <c r="B1846" t="s">
-        <v>1866</v>
+        <v>2451</v>
       </c>
       <c r="C1846" t="s">
         <v>281</v>
       </c>
       <c r="D1846">
-        <v>1845</v>
+        <v>1025</v>
       </c>
       <c r="E1846" t="s">
-        <v>838</v>
+        <v>1347</v>
       </c>
     </row>
     <row r="1847" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
@@ -67575,21 +67575,21 @@
         <v>650</v>
       </c>
     </row>
-    <row r="1851" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
+    <row r="1851" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A1851" t="s">
-        <v>4189</v>
+        <v>803</v>
       </c>
       <c r="B1851" t="s">
-        <v>4190</v>
+        <v>804</v>
       </c>
       <c r="C1851" t="s">
         <v>281</v>
       </c>
       <c r="D1851">
-        <v>1850</v>
+        <v>304</v>
       </c>
       <c r="E1851" t="s">
-        <v>986</v>
+        <v>805</v>
       </c>
     </row>
     <row r="1852" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
@@ -67728,21 +67728,21 @@
         <v>717</v>
       </c>
     </row>
-    <row r="1860" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
+    <row r="1860" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A1860" t="s">
-        <v>4208</v>
+        <v>490</v>
       </c>
       <c r="B1860" t="s">
-        <v>4209</v>
+        <v>491</v>
       </c>
       <c r="C1860" t="s">
         <v>281</v>
       </c>
       <c r="D1860">
-        <v>1859</v>
+        <v>186</v>
       </c>
       <c r="E1860" t="s">
-        <v>3900</v>
+        <v>484</v>
       </c>
     </row>
     <row r="1861" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
@@ -68391,21 +68391,21 @@
         <v>791</v>
       </c>
     </row>
-    <row r="1899" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
+    <row r="1899" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A1899" t="s">
-        <v>4290</v>
+        <v>1829</v>
       </c>
       <c r="B1899" t="s">
-        <v>4291</v>
+        <v>1830</v>
       </c>
       <c r="C1899" t="s">
         <v>281</v>
       </c>
       <c r="D1899">
-        <v>1898</v>
+        <v>740</v>
       </c>
       <c r="E1899" t="s">
-        <v>2109</v>
+        <v>484</v>
       </c>
     </row>
     <row r="1900" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
@@ -69292,7 +69292,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="1952" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="1952" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A1952" t="s">
         <v>4402</v>
       </c>
@@ -69411,7 +69411,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="1959" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="1959" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A1959" t="s">
         <v>4417</v>
       </c>
@@ -69496,7 +69496,7 @@
         <v>1078</v>
       </c>
     </row>
-    <row r="1964" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="1964" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A1964" t="s">
         <v>4427</v>
       </c>
@@ -69785,7 +69785,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="1981" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="1981" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A1981" t="s">
         <v>4463</v>
       </c>
@@ -70363,7 +70363,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="2015" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="2015" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A2015" t="s">
         <v>4534</v>
       </c>
@@ -71621,7 +71621,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="2089" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="2089" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A2089" t="s">
         <v>4691</v>
       </c>
@@ -71944,7 +71944,7 @@
         <v>791</v>
       </c>
     </row>
-    <row r="2108" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="2108" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A2108" t="s">
         <v>4732</v>
       </c>
@@ -71961,7 +71961,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="2109" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="2109" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A2109" t="s">
         <v>4734</v>
       </c>
@@ -72556,21 +72556,21 @@
         <v>40</v>
       </c>
     </row>
-    <row r="2144" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
+    <row r="2144" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A2144" t="s">
-        <v>4806</v>
+        <v>635</v>
       </c>
       <c r="B2144" t="s">
-        <v>4807</v>
+        <v>636</v>
       </c>
       <c r="C2144" t="s">
         <v>281</v>
       </c>
       <c r="D2144">
-        <v>2143</v>
+        <v>244</v>
       </c>
       <c r="E2144" t="s">
-        <v>27</v>
+        <v>637</v>
       </c>
     </row>
     <row r="2145" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
@@ -72692,21 +72692,21 @@
         <v>40</v>
       </c>
     </row>
-    <row r="2152" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
+    <row r="2152" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A2152" t="s">
-        <v>4822</v>
+        <v>608</v>
       </c>
       <c r="B2152" t="s">
-        <v>4823</v>
+        <v>609</v>
       </c>
       <c r="C2152" t="s">
         <v>281</v>
       </c>
       <c r="D2152">
-        <v>2151</v>
+        <v>234</v>
       </c>
       <c r="E2152" t="s">
-        <v>650</v>
+        <v>610</v>
       </c>
     </row>
     <row r="2153" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
@@ -72760,21 +72760,21 @@
         <v>247</v>
       </c>
     </row>
-    <row r="2156" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
+    <row r="2156" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A2156" t="s">
-        <v>4830</v>
+        <v>1884</v>
       </c>
       <c r="B2156" t="s">
-        <v>4831</v>
+        <v>1885</v>
       </c>
       <c r="C2156" t="s">
         <v>281</v>
       </c>
       <c r="D2156">
-        <v>2155</v>
+        <v>766</v>
       </c>
       <c r="E2156" t="s">
-        <v>640</v>
+        <v>610</v>
       </c>
     </row>
     <row r="2157" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
@@ -72862,7 +72862,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2162" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="2162" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A2162" t="s">
         <v>4843</v>
       </c>
@@ -72964,7 +72964,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2168" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="2168" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A2168" t="s">
         <v>4856</v>
       </c>
@@ -73372,7 +73372,7 @@
         <v>1785</v>
       </c>
     </row>
-    <row r="2192" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="2192" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A2192" t="s">
         <v>4906</v>
       </c>
@@ -73678,7 +73678,7 @@
         <v>606</v>
       </c>
     </row>
-    <row r="2210" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="2210" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A2210" t="s">
         <v>4944</v>
       </c>
@@ -73695,21 +73695,21 @@
         <v>668</v>
       </c>
     </row>
-    <row r="2211" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
+    <row r="2211" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A2211" t="s">
-        <v>4946</v>
+        <v>827</v>
       </c>
       <c r="B2211" t="s">
-        <v>4947</v>
+        <v>828</v>
       </c>
       <c r="C2211" t="s">
         <v>281</v>
       </c>
       <c r="D2211">
-        <v>2210</v>
+        <v>313</v>
       </c>
       <c r="E2211" t="s">
-        <v>4701</v>
+        <v>829</v>
       </c>
     </row>
     <row r="2212" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
@@ -73967,7 +73967,7 @@
         <v>1078</v>
       </c>
     </row>
-    <row r="2227" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="2227" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A2227" t="s">
         <v>4979</v>
       </c>
@@ -74562,7 +74562,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="2262" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="2262" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A2262" t="s">
         <v>5051</v>
       </c>
@@ -74715,7 +74715,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="2271" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="2271" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A2271" t="s">
         <v>5069</v>
       </c>
@@ -75297,10 +75297,12 @@
   <autoFilter ref="A1:E2304" xr:uid="{00000000-0001-0000-0000-000000000000}">
     <filterColumn colId="2">
       <filters>
-        <filter val="한국경제"/>
-        <filter val="한국경제매거진"/>
+        <filter val="물류신문"/>
       </filters>
     </filterColumn>
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A102:E2211">
+      <sortCondition descending="1" ref="E1:E2304"/>
+    </sortState>
   </autoFilter>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>